<commit_message>
data drawdown dates fixed
</commit_message>
<xml_diff>
--- a/drawdown_list.xlsx
+++ b/drawdown_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh\Desktop\drawdown-vis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{370B1862-A4DC-4A61-A70A-F0FC5A0FE14D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47D8E7B-8DB3-42E2-8EE3-E50FBB4862CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2FAE9D53-CD47-4F4F-9902-429DF056ABF0}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +452,7 @@
         <v>-0.1004</v>
       </c>
       <c r="D2" s="1">
-        <v>33014</v>
+        <v>32905</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -466,7 +466,7 @@
         <v>-0.1918</v>
       </c>
       <c r="D3" s="1">
-        <v>33280</v>
+        <v>33161</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -480,7 +480,7 @@
         <v>-0.1075</v>
       </c>
       <c r="D4" s="1">
-        <v>35769</v>
+        <v>35732</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -494,7 +494,7 @@
         <v>-0.19189999999999999</v>
       </c>
       <c r="D5" s="1">
-        <v>36122</v>
+        <v>36039</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -508,7 +508,7 @@
         <v>-0.11799999999999999</v>
       </c>
       <c r="D6" s="1">
-        <v>36480</v>
+        <v>36452</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -522,7 +522,7 @@
         <v>-0.1114</v>
       </c>
       <c r="D7" s="1">
-        <v>36770</v>
+        <v>36633</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -536,7 +536,7 @@
         <v>-0.47410000000000002</v>
       </c>
       <c r="D8" s="1">
-        <v>39013</v>
+        <v>37546</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -550,7 +550,7 @@
         <v>-0.55249999999999999</v>
       </c>
       <c r="D9" s="1">
-        <v>41001</v>
+        <v>39888</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -564,7 +564,7 @@
         <v>-0.12959999999999999</v>
       </c>
       <c r="D10" s="1">
-        <v>42478</v>
+        <v>42417</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
raw data error fixed
</commit_message>
<xml_diff>
--- a/drawdown_list.xlsx
+++ b/drawdown_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh\Desktop\drawdown-vis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47D8E7B-8DB3-42E2-8EE3-E50FBB4862CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FFA367-A7E9-4552-A70F-4D65C3A2FD21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2FAE9D53-CD47-4F4F-9902-429DF056ABF0}"/>
   </bookViews>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C170FF-D92C-4A01-82EF-DD5F7346B9EC}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,99 +513,85 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>36612</v>
+        <v>36774</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>529</v>
       </c>
       <c r="C7" s="2">
-        <v>-0.1114</v>
+        <v>-0.47410000000000002</v>
       </c>
       <c r="D7" s="1">
-        <v>36633</v>
+        <v>37546</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>36774</v>
+        <v>39365</v>
       </c>
       <c r="B8">
-        <v>529</v>
+        <v>355</v>
       </c>
       <c r="C8" s="2">
-        <v>-0.47410000000000002</v>
+        <v>-0.55249999999999999</v>
       </c>
       <c r="D8" s="1">
-        <v>37546</v>
+        <v>39888</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>39365</v>
+        <v>42206</v>
       </c>
       <c r="B9">
-        <v>355</v>
+        <v>143</v>
       </c>
       <c r="C9" s="2">
-        <v>-0.55249999999999999</v>
+        <v>-0.12959999999999999</v>
       </c>
       <c r="D9" s="1">
-        <v>39888</v>
+        <v>42417</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>42206</v>
+        <v>43126</v>
       </c>
       <c r="B10">
-        <v>143</v>
-      </c>
-      <c r="C10" s="2">
-        <v>-0.12959999999999999</v>
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="D10" s="1">
-        <v>42417</v>
+        <v>43139</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>43126</v>
+        <v>43363</v>
       </c>
       <c r="B11">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
+        <v>63</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-0.19800000000000001</v>
       </c>
       <c r="D11" s="1">
-        <v>43139</v>
+        <v>43458</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>43363</v>
+        <v>43880</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2">
-        <v>-0.19800000000000001</v>
+        <v>-0.31900000000000001</v>
       </c>
       <c r="D12" s="1">
-        <v>43458</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>43880</v>
-      </c>
-      <c r="B13">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2">
-        <v>-0.31900000000000001</v>
-      </c>
-      <c r="D13" s="1">
         <v>43910</v>
       </c>
     </row>

</xml_diff>

<commit_message>
labels and colors added
</commit_message>
<xml_diff>
--- a/drawdown_list.xlsx
+++ b/drawdown_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh\Desktop\drawdown-vis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FFA367-A7E9-4552-A70F-4D65C3A2FD21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D62BBC-73D0-4375-9110-3B6C94EEA886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2FAE9D53-CD47-4F4F-9902-429DF056ABF0}"/>
   </bookViews>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C170FF-D92C-4A01-82EF-DD5F7346B9EC}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,155 +443,141 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>32876</v>
+        <v>33071</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2">
-        <v>-0.1004</v>
+        <v>-0.1918</v>
       </c>
       <c r="D2" s="1">
-        <v>32905</v>
+        <v>33161</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>33071</v>
+        <v>35711</v>
       </c>
       <c r="B3">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2">
-        <v>-0.1918</v>
+        <v>-0.1075</v>
       </c>
       <c r="D3" s="1">
-        <v>33161</v>
+        <v>35732</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>35711</v>
+        <v>35996</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2">
-        <v>-0.1075</v>
+        <v>-0.19189999999999999</v>
       </c>
       <c r="D4" s="1">
-        <v>35732</v>
+        <v>36039</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>35996</v>
+        <v>36360</v>
       </c>
       <c r="B5">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2">
-        <v>-0.19189999999999999</v>
+        <v>-0.11799999999999999</v>
       </c>
       <c r="D5" s="1">
-        <v>36039</v>
+        <v>36452</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>36360</v>
+        <v>36774</v>
       </c>
       <c r="B6">
-        <v>64</v>
+        <v>529</v>
       </c>
       <c r="C6" s="2">
-        <v>-0.11799999999999999</v>
+        <v>-0.47410000000000002</v>
       </c>
       <c r="D6" s="1">
-        <v>36452</v>
+        <v>37546</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>36774</v>
+        <v>39365</v>
       </c>
       <c r="B7">
-        <v>529</v>
+        <v>355</v>
       </c>
       <c r="C7" s="2">
-        <v>-0.47410000000000002</v>
+        <v>-0.55249999999999999</v>
       </c>
       <c r="D7" s="1">
-        <v>37546</v>
+        <v>39888</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>39365</v>
+        <v>42206</v>
       </c>
       <c r="B8">
-        <v>355</v>
+        <v>143</v>
       </c>
       <c r="C8" s="2">
-        <v>-0.55249999999999999</v>
+        <v>-0.12959999999999999</v>
       </c>
       <c r="D8" s="1">
-        <v>39888</v>
+        <v>42417</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>42206</v>
+        <v>43126</v>
       </c>
       <c r="B9">
-        <v>143</v>
-      </c>
-      <c r="C9" s="2">
-        <v>-0.12959999999999999</v>
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>42417</v>
+        <v>43139</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>43126</v>
+        <v>43363</v>
       </c>
       <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
+        <v>63</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-0.19800000000000001</v>
       </c>
       <c r="D10" s="1">
-        <v>43139</v>
+        <v>43458</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>43363</v>
+        <v>43880</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2">
-        <v>-0.19800000000000001</v>
+        <v>-0.31900000000000001</v>
       </c>
       <c r="D11" s="1">
-        <v>43458</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>43880</v>
-      </c>
-      <c r="B12">
-        <v>30</v>
-      </c>
-      <c r="C12" s="2">
-        <v>-0.31900000000000001</v>
-      </c>
-      <c r="D12" s="1">
         <v>43910</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed a redundant data point
</commit_message>
<xml_diff>
--- a/drawdown_list.xlsx
+++ b/drawdown_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh\Desktop\drawdown-vis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D62BBC-73D0-4375-9110-3B6C94EEA886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5946A1E6-CBA9-4D55-B074-259A56FF6A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2FAE9D53-CD47-4F4F-9902-429DF056ABF0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Drawdown Start</t>
   </si>
@@ -46,22 +46,12 @@
   <si>
     <t>Drawdown Conclusion</t>
   </si>
-  <si>
-    <t>‐10.20%</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,21 +77,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -413,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C170FF-D92C-4A01-82EF-DD5F7346B9EC}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,43 +526,29 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>43126</v>
+        <v>43363</v>
       </c>
       <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
+        <v>63</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-0.19800000000000001</v>
       </c>
       <c r="D9" s="1">
-        <v>43139</v>
+        <v>43458</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>43363</v>
+        <v>43880</v>
       </c>
       <c r="B10">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2">
-        <v>-0.19800000000000001</v>
+        <v>-0.31900000000000001</v>
       </c>
       <c r="D10" s="1">
-        <v>43458</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>43880</v>
-      </c>
-      <c r="B11">
-        <v>30</v>
-      </c>
-      <c r="C11" s="2">
-        <v>-0.31900000000000001</v>
-      </c>
-      <c r="D11" s="1">
         <v>43910</v>
       </c>
     </row>

</xml_diff>